<commit_message>
Se cambio la edad de ana y se cambio la provincia de luis
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\conflicto-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CA9D33-36FA-409D-B122-985F2EEC9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6AC311-5C9C-41E3-9EEE-DACD3D032BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FDAAAD7-8DD7-407A-BDC0-F1D1B524D643}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Luis</t>
   </si>
   <si>
-    <t>Alajuela</t>
+    <t>Guanacaste</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Se actualizo la edad de ana y la prinvincia donde vive luis
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\conflicto-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CA9D33-36FA-409D-B122-985F2EEC9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D52A62-3EDD-4740-AF0A-AB668969F8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FDAAAD7-8DD7-407A-BDC0-F1D1B524D643}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Luis</t>
   </si>
   <si>
-    <t>Alajuela</t>
+    <t>Cartago</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
se actualizado los datos conforme a como estan en el main
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\conflicto-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D52A62-3EDD-4740-AF0A-AB668969F8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09229DC4-FF97-43FD-B182-349F53A2E7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FDAAAD7-8DD7-407A-BDC0-F1D1B524D643}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Luis</t>
   </si>
   <si>
-    <t>Cartago</t>
+    <t>Guanacaste</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
se actualizado la rama conforme a como esta en main
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjcl-\Desktop\conflicto-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09229DC4-FF97-43FD-B182-349F53A2E7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80D0725-2D0E-440B-B9D0-63000149E63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FDAAAD7-8DD7-407A-BDC0-F1D1B524D643}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>